<commit_message>
More work on update
</commit_message>
<xml_diff>
--- a/LaTeX/PreliminaryWork/Graphs/BuretteVsSyringe.xlsx
+++ b/LaTeX/PreliminaryWork/Graphs/BuretteVsSyringe.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
   <si>
     <t>Time (s)</t>
   </si>
@@ -41,11 +41,17 @@
   <si>
     <t>Repeat 3</t>
   </si>
+  <si>
+    <t>Average</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -238,15 +244,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -266,6 +268,20 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -377,7 +393,7 @@
             <c:numRef>
               <c:f>Sheet1!$D$5:$D$15</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -469,7 +485,7 @@
             <c:numRef>
               <c:f>Sheet1!$E$5:$E$15</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0.5</c:v>
@@ -561,7 +577,7 @@
             <c:numRef>
               <c:f>Sheet1!$F$5:$F$15</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -611,11 +627,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="67146880"/>
-        <c:axId val="67148800"/>
+        <c:axId val="152529152"/>
+        <c:axId val="152535424"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="67146880"/>
+        <c:axId val="152529152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -646,7 +662,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67148800"/>
+        <c:crossAx val="152535424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -654,7 +670,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="67148800"/>
+        <c:axId val="152535424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -680,11 +696,11 @@
           <c:layout/>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67146880"/>
+        <c:crossAx val="152529152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -812,7 +828,7 @@
             <c:numRef>
               <c:f>Sheet1!$J$5:$J$15</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -904,7 +920,7 @@
             <c:numRef>
               <c:f>Sheet1!$K$5:$K$15</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -996,7 +1012,7 @@
             <c:numRef>
               <c:f>Sheet1!$L$5:$L$15</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -1046,11 +1062,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="67200128"/>
-        <c:axId val="67202048"/>
+        <c:axId val="153159936"/>
+        <c:axId val="153166208"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="67200128"/>
+        <c:axId val="153159936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1081,7 +1097,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67202048"/>
+        <c:crossAx val="153166208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1089,7 +1105,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="67202048"/>
+        <c:axId val="153166208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1115,11 +1131,11 @@
           <c:layout/>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67200128"/>
+        <c:crossAx val="153159936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1503,22 +1519,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:L16"/>
+  <dimension ref="B1:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AE30" sqref="AE30"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="10.42578125" customWidth="1"/>
-    <col min="5" max="6" width="11" customWidth="1"/>
+    <col min="5" max="5" width="11" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" customWidth="1"/>
     <col min="10" max="10" width="11.42578125" customWidth="1"/>
     <col min="11" max="11" width="11.85546875" customWidth="1"/>
     <col min="12" max="12" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:13" x14ac:dyDescent="0.25">
       <c r="E1" t="s">
         <v>1</v>
       </c>
@@ -1526,345 +1543,441 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="2:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="11"/>
-      <c r="D3" s="8" t="s">
+    <row r="2" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="7"/>
+      <c r="D3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="9"/>
-      <c r="F3" s="10"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="15" t="s">
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="6"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="9"/>
-      <c r="L3" s="10"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="6"/>
     </row>
-    <row r="4" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="1"/>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="G4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="J4" s="12" t="s">
+      <c r="J4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="K4" s="13" t="s">
+      <c r="K4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="L4" s="14" t="s">
+      <c r="L4" s="10" t="s">
         <v>7</v>
       </c>
+      <c r="M4" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="5" spans="2:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="1"/>
-      <c r="C5" s="6">
+      <c r="C5" s="2">
         <v>0</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="12">
         <v>0</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="13">
         <v>0.5</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="13">
         <v>0</v>
       </c>
-      <c r="I5" s="6">
+      <c r="G5" s="20">
+        <f>(D5+E5+F5)/3</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I5" s="2">
         <v>0</v>
       </c>
-      <c r="J5" s="4">
+      <c r="J5" s="16">
         <v>0</v>
       </c>
-      <c r="K5" s="5">
+      <c r="K5" s="17">
         <v>0</v>
       </c>
-      <c r="L5" s="5">
+      <c r="L5" s="17">
         <v>0</v>
       </c>
+      <c r="M5" s="21">
+        <f>(J5+K5+L5)/3</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="2:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="1"/>
-      <c r="C6" s="6">
+      <c r="C6" s="2">
         <v>30</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="14">
         <v>1</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="15">
         <v>2</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="15">
         <v>1.5</v>
       </c>
-      <c r="I6" s="6">
+      <c r="G6" s="20">
+        <f t="shared" ref="G6:G15" si="0">(D6+E6+F6)/3</f>
+        <v>1.5</v>
+      </c>
+      <c r="I6" s="2">
         <v>30</v>
       </c>
-      <c r="J6" s="3">
+      <c r="J6" s="18">
         <v>0.75</v>
       </c>
-      <c r="K6" s="2">
+      <c r="K6" s="19">
         <v>1.35</v>
       </c>
-      <c r="L6" s="2">
+      <c r="L6" s="19">
         <v>0.95</v>
       </c>
+      <c r="M6" s="21">
+        <f t="shared" ref="M6:M15" si="1">(J6+K6+L6)/3</f>
+        <v>1.0166666666666666</v>
+      </c>
     </row>
-    <row r="7" spans="2:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="1"/>
-      <c r="C7" s="6">
+      <c r="C7" s="2">
         <v>60</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="14">
         <v>2.5</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="15">
         <v>3.5</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="15">
         <v>3</v>
       </c>
-      <c r="I7" s="6">
+      <c r="G7" s="20">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="I7" s="2">
         <v>60</v>
       </c>
-      <c r="J7" s="3">
+      <c r="J7" s="18">
         <v>1.65</v>
       </c>
-      <c r="K7" s="2">
+      <c r="K7" s="19">
         <v>3</v>
       </c>
-      <c r="L7" s="2">
+      <c r="L7" s="19">
         <v>2.0499999999999998</v>
       </c>
+      <c r="M7" s="21">
+        <f t="shared" si="1"/>
+        <v>2.2333333333333334</v>
+      </c>
     </row>
-    <row r="8" spans="2:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="1"/>
-      <c r="C8" s="6">
+      <c r="C8" s="2">
         <v>90</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="14">
         <v>4</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="15">
         <v>5</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="15">
         <v>4.5</v>
       </c>
-      <c r="I8" s="6">
+      <c r="G8" s="20">
+        <f t="shared" si="0"/>
+        <v>4.5</v>
+      </c>
+      <c r="I8" s="2">
         <v>90</v>
       </c>
-      <c r="J8" s="3">
+      <c r="J8" s="18">
         <v>2.5499999999999998</v>
       </c>
-      <c r="K8" s="2">
+      <c r="K8" s="19">
         <v>4.95</v>
       </c>
-      <c r="L8" s="2">
+      <c r="L8" s="19">
         <v>3.25</v>
       </c>
+      <c r="M8" s="21">
+        <f t="shared" si="1"/>
+        <v>3.5833333333333335</v>
+      </c>
     </row>
-    <row r="9" spans="2:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="1"/>
-      <c r="C9" s="6">
+      <c r="C9" s="2">
         <v>120</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="14">
         <v>6</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="15">
         <v>6.5</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="15">
         <v>6.5</v>
       </c>
-      <c r="I9" s="6">
+      <c r="G9" s="20">
+        <f t="shared" si="0"/>
+        <v>6.333333333333333</v>
+      </c>
+      <c r="I9" s="2">
         <v>120</v>
       </c>
-      <c r="J9" s="3">
+      <c r="J9" s="18">
         <v>3.25</v>
       </c>
-      <c r="K9" s="2">
+      <c r="K9" s="19">
         <v>6.45</v>
       </c>
-      <c r="L9" s="2">
+      <c r="L9" s="19">
         <v>5.05</v>
       </c>
+      <c r="M9" s="21">
+        <f t="shared" si="1"/>
+        <v>4.916666666666667</v>
+      </c>
     </row>
-    <row r="10" spans="2:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="1"/>
-      <c r="C10" s="6">
+      <c r="C10" s="2">
         <v>150</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="14">
         <v>7.5</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="15">
         <v>8</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="15">
         <v>8</v>
       </c>
-      <c r="I10" s="6">
+      <c r="G10" s="20">
+        <f t="shared" si="0"/>
+        <v>7.833333333333333</v>
+      </c>
+      <c r="I10" s="2">
         <v>150</v>
       </c>
-      <c r="J10" s="3">
+      <c r="J10" s="18">
         <v>3.9</v>
       </c>
-      <c r="K10" s="2">
+      <c r="K10" s="19">
         <v>7.85</v>
       </c>
-      <c r="L10" s="2">
+      <c r="L10" s="19">
         <v>6.8</v>
       </c>
+      <c r="M10" s="21">
+        <f t="shared" si="1"/>
+        <v>6.1833333333333336</v>
+      </c>
     </row>
-    <row r="11" spans="2:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="1"/>
-      <c r="C11" s="6">
+      <c r="C11" s="2">
         <v>180</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="14">
         <v>9.5</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="15">
         <v>10</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="15">
         <v>9.5</v>
       </c>
-      <c r="I11" s="6">
+      <c r="G11" s="20">
+        <f t="shared" si="0"/>
+        <v>9.6666666666666661</v>
+      </c>
+      <c r="I11" s="2">
         <v>180</v>
       </c>
-      <c r="J11" s="3">
+      <c r="J11" s="18">
         <v>4.8499999999999996</v>
       </c>
-      <c r="K11" s="2">
+      <c r="K11" s="19">
         <v>8.3000000000000007</v>
       </c>
-      <c r="L11" s="2">
+      <c r="L11" s="19">
         <v>7.9</v>
       </c>
+      <c r="M11" s="21">
+        <f t="shared" si="1"/>
+        <v>7.0166666666666666</v>
+      </c>
     </row>
-    <row r="12" spans="2:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="1"/>
-      <c r="C12" s="6">
+      <c r="C12" s="2">
         <v>210</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="14">
         <v>11.5</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="15">
         <v>12</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="15">
         <v>11.5</v>
       </c>
-      <c r="I12" s="6">
+      <c r="G12" s="20">
+        <f t="shared" si="0"/>
+        <v>11.666666666666666</v>
+      </c>
+      <c r="I12" s="2">
         <v>210</v>
       </c>
-      <c r="J12" s="3">
+      <c r="J12" s="18">
         <v>5.9</v>
       </c>
-      <c r="K12" s="2">
+      <c r="K12" s="19">
         <v>10.25</v>
       </c>
-      <c r="L12" s="2">
+      <c r="L12" s="19">
         <v>8.15</v>
       </c>
+      <c r="M12" s="21">
+        <f t="shared" si="1"/>
+        <v>8.1</v>
+      </c>
     </row>
-    <row r="13" spans="2:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="1"/>
-      <c r="C13" s="6">
+      <c r="C13" s="2">
         <v>240</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="14">
         <v>13</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="15">
         <v>14</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" s="15">
         <v>13.5</v>
       </c>
-      <c r="I13" s="6">
+      <c r="G13" s="20">
+        <f t="shared" si="0"/>
+        <v>13.5</v>
+      </c>
+      <c r="I13" s="2">
         <v>240</v>
       </c>
-      <c r="J13" s="3">
+      <c r="J13" s="18">
         <v>7.15</v>
       </c>
-      <c r="K13" s="2">
+      <c r="K13" s="19">
         <v>11.1</v>
       </c>
-      <c r="L13" s="2">
+      <c r="L13" s="19">
         <v>10.199999999999999</v>
       </c>
+      <c r="M13" s="21">
+        <f t="shared" si="1"/>
+        <v>9.4833333333333325</v>
+      </c>
     </row>
-    <row r="14" spans="2:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="1"/>
-      <c r="C14" s="6">
+      <c r="C14" s="2">
         <v>270</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="14">
         <v>14.5</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="15">
         <v>15.5</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="15">
         <v>15</v>
       </c>
-      <c r="I14" s="6">
+      <c r="G14" s="20">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="I14" s="2">
         <v>270</v>
       </c>
-      <c r="J14" s="3">
+      <c r="J14" s="18">
         <v>9</v>
       </c>
-      <c r="K14" s="2">
+      <c r="K14" s="19">
         <v>11.9</v>
       </c>
-      <c r="L14" s="2">
+      <c r="L14" s="19">
         <v>11.35</v>
       </c>
+      <c r="M14" s="21">
+        <f t="shared" si="1"/>
+        <v>10.75</v>
+      </c>
     </row>
-    <row r="15" spans="2:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="6">
+    <row r="15" spans="2:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C15" s="2">
         <v>300</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="14">
         <v>16</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="15">
         <v>17.5</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15" s="15">
         <v>17</v>
       </c>
-      <c r="I15" s="6">
+      <c r="G15" s="20">
+        <f t="shared" si="0"/>
+        <v>16.833333333333332</v>
+      </c>
+      <c r="I15" s="2">
         <v>300</v>
       </c>
-      <c r="J15" s="3">
+      <c r="J15" s="18">
         <v>10.45</v>
       </c>
-      <c r="K15" s="2">
+      <c r="K15" s="19">
         <v>12.65</v>
       </c>
-      <c r="L15" s="2">
+      <c r="L15" s="19">
         <v>13.5</v>
       </c>
+      <c r="M15" s="21">
+        <f t="shared" si="1"/>
+        <v>12.200000000000001</v>
+      </c>
     </row>
-    <row r="16" spans="2:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="2:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>